<commit_message>
Anotacoes gerais para o grupo
</commit_message>
<xml_diff>
--- a/CupcakeriaOnline/Documentos/modelo.xlsx
+++ b/CupcakeriaOnline/Documentos/modelo.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Fábio\IFSP\6º Semestre\A6LP2\_Trabalho\Projeto\CupcakeriaOnline\CupcakeriaOnline\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Anotacoes" sheetId="2" r:id="rId1"/>
+    <sheet name="Tabelas" sheetId="1" r:id="rId2"/>
+    <sheet name="Definicoes" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
   <si>
     <t>Cliente</t>
   </si>
@@ -189,13 +191,49 @@
   </si>
   <si>
     <t>dispCobertura</t>
+  </si>
+  <si>
+    <t>Divisão para criação das Models/Repositories:</t>
+  </si>
+  <si>
+    <t>Utilizar o mesmo nome da tabela para as models</t>
+  </si>
+  <si>
+    <t>E o mesmo nome dos campos para os atributos</t>
+  </si>
+  <si>
+    <t>Fábio</t>
+  </si>
+  <si>
+    <t>André</t>
+  </si>
+  <si>
+    <t>Artur</t>
+  </si>
+  <si>
+    <t>Vitor</t>
+  </si>
+  <si>
+    <t>Link do OneDrive da Aline:</t>
+  </si>
+  <si>
+    <t>1drv.ms/1Trd0ro</t>
+  </si>
+  <si>
+    <t>Importações de arquivos no projeto</t>
+  </si>
+  <si>
+    <t>Formatos: xml e csv</t>
+  </si>
+  <si>
+    <t>Tabela: Endereço</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +249,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -220,7 +266,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -228,13 +274,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +674,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,200 +796,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="10" t="s">
         <v>54</v>
       </c>
     </row>
@@ -733,4 +997,37 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Alterando documentacao e alterando arquivo do projeto
Alterando documentacao e alterando arquivo do projeto
</commit_message>
<xml_diff>
--- a/CupcakeriaOnline/Documentos/modelo.xlsx
+++ b/CupcakeriaOnline/Documentos/modelo.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Fábio\IFSP\6º Semestre\A6LP2\_Trabalho\Projeto\CupcakeriaOnline\CupcakeriaOnline\Documentos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Anotacoes" sheetId="2" r:id="rId1"/>
     <sheet name="Tabelas" sheetId="1" r:id="rId2"/>
     <sheet name="Definicoes" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>Cliente</t>
   </si>
@@ -227,6 +222,9 @@
   </si>
   <si>
     <t>Tabela: Endereço</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
   </si>
 </sst>
 </file>
@@ -666,7 +664,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -674,17 +672,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -692,12 +693,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +706,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -713,7 +714,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -721,7 +722,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -729,15 +730,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -745,7 +749,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -753,7 +757,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -761,12 +765,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Adicionado arquivos no projeto
Adicionado arquivos no projeto
</commit_message>
<xml_diff>
--- a/CupcakeriaOnline/Documentos/modelo.xlsx
+++ b/CupcakeriaOnline/Documentos/modelo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Anotacoes" sheetId="2" r:id="rId1"/>
@@ -661,7 +661,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -671,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adicionado classe Model Cupcake_Pedido
Adicionado classe Model Cupcake_Pedido
</commit_message>
<xml_diff>
--- a/CupcakeriaOnline/Documentos/modelo.xlsx
+++ b/CupcakeriaOnline/Documentos/modelo.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artur\Documents\GitHub\cupcakeria\CupcakeriaOnline\Documentos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Anotacoes" sheetId="2" r:id="rId1"/>
@@ -228,7 +233,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,14 +243,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -388,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,7 +658,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -671,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Alteração na planilha de controle tarefas
Alteração na planilha de controle tarefas
</commit_message>
<xml_diff>
--- a/CupcakeriaOnline/Documentos/modelo.xlsx
+++ b/CupcakeriaOnline/Documentos/modelo.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>Cliente</t>
   </si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t>Tabela: Endereço</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>View</t>
   </si>
 </sst>
 </file>
@@ -373,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -386,6 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,20 +676,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -687,12 +699,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,7 +712,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -708,7 +720,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -716,31 +728,46 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -748,7 +775,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -756,12 +783,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Novas tarefas para entrega
</commit_message>
<xml_diff>
--- a/CupcakeriaOnline/Documentos/modelo.xlsx
+++ b/CupcakeriaOnline/Documentos/modelo.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artur\Documents\GitHub\cupcakeria\CupcakeriaOnline\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Fabio\IFSP\6º Semestre\A6LP2\_Trabalho\Repositório\CupcakeriaOnline\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Anotacoes" sheetId="2" r:id="rId1"/>
-    <sheet name="Tabelas" sheetId="1" r:id="rId2"/>
-    <sheet name="Definicoes" sheetId="4" r:id="rId3"/>
+    <sheet name="NOVO - Tarefas" sheetId="5" r:id="rId1"/>
+    <sheet name="Anotacoes" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelas" sheetId="1" r:id="rId3"/>
+    <sheet name="Definicoes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
   <si>
     <t>Cliente</t>
   </si>
@@ -236,6 +237,54 @@
   </si>
   <si>
     <t>View</t>
+  </si>
+  <si>
+    <t>cadastrar nova massa (administrador)</t>
+  </si>
+  <si>
+    <t>cadastrar nova cobertura (administrador)</t>
+  </si>
+  <si>
+    <t>cadastrar novo recheio (administrador)</t>
+  </si>
+  <si>
+    <t>Cadastrar novo perfil (usuário)</t>
+  </si>
+  <si>
+    <t>Cadastrar novo endereço (usuário)</t>
+  </si>
+  <si>
+    <t>cadastrar novo cupcake_pedido (adicionar ao carrinho)</t>
+  </si>
+  <si>
+    <t>cadastrar novo pedido (finalizar compra com varios cupcake_pedido)</t>
+  </si>
+  <si>
+    <t>Relatório ADM: ver status de todos os pedidos feitos até o momento</t>
+  </si>
+  <si>
+    <t>Relatório ADM: ver massa mais comprada até hoje</t>
+  </si>
+  <si>
+    <t>Relatório ADM: ver cobertura mais comprada até hoje</t>
+  </si>
+  <si>
+    <t>Relatório ADM: ver recheio mais comprado até hoje</t>
+  </si>
+  <si>
+    <t>Relatório USU: Ver histórico de pedidos</t>
+  </si>
+  <si>
+    <t>Adicional:</t>
+  </si>
+  <si>
+    <t>Scripts sql para criar banco e inserir dados</t>
+  </si>
+  <si>
+    <t>Importar arquivo de novo endereço (.csv) + possibilidade de editar dados antes de gravar</t>
+  </si>
+  <si>
+    <t>Importar arquivo de novo endereço (.xml) + possibilidade de editar dados antes de gravar</t>
   </si>
 </sst>
 </file>
@@ -676,9 +725,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="82.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -799,7 +946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
@@ -1021,7 +1168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>

</xml_diff>

<commit_message>
link para criar filters
</commit_message>
<xml_diff>
--- a/CupcakeriaOnline/Documentos/modelo.xlsx
+++ b/CupcakeriaOnline/Documentos/modelo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Fabio\IFSP\6º Semestre\A6LP2\_Trabalho\Repositório\CupcakeriaOnline\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Source\Repos\cupcakeria\CupcakeriaOnline\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NOVO - Tarefas" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
   <si>
     <t>Cliente</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>Página de login</t>
+  </si>
+  <si>
+    <t>fk_idPedido</t>
+  </si>
+  <si>
+    <t>// http://www.macoratti.net/13/12/mvc_ddl2.htm</t>
   </si>
 </sst>
 </file>
@@ -440,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -454,6 +460,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,10 +982,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,6 +1105,9 @@
       <c r="D6" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="E6" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="F6" s="5" t="s">
         <v>32</v>
       </c>
@@ -1187,6 +1197,11 @@
       </c>
       <c r="C16" s="10" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>